<commit_message>
Changes in Corporate Profile pages
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>admin@123</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>212</t>
+  </si>
+  <si>
+    <t>246</t>
+  </si>
+  <si>
+    <t>366</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1075,7 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WS Admin Invite Scripts II
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView windowHeight="7605" windowWidth="16020" xWindow="0" yWindow="2445"/>
+    <workbookView activeTab="4" firstSheet="2" windowHeight="3540" windowWidth="12000" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" r:id="rId1" sheetId="1"/>
@@ -14,7 +14,7 @@
     <sheet name="Write data" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K23"/>
+  <oleSize ref="A1:K16"/>
 </workbook>
 </file>
 
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="143">
   <si>
     <t>admin@123</t>
   </si>
@@ -196,9 +196,6 @@
     <t>register@mailinator.com</t>
   </si>
   <si>
-    <t>shub@mailinator.com</t>
-  </si>
-  <si>
     <t>Job ID</t>
   </si>
   <si>
@@ -208,52 +205,283 @@
     <t>AdminPassword</t>
   </si>
   <si>
-    <t>admin@workstreets.com</t>
-  </si>
-  <si>
     <t>Agency Email</t>
   </si>
   <si>
-    <t>first@mailinator.com</t>
-  </si>
-  <si>
     <t>Agency Password</t>
   </si>
   <si>
     <t>Software Regression Engineer</t>
   </si>
   <si>
-    <t>178</t>
+    <t>Candidate Email</t>
+  </si>
+  <si>
+    <t>sathish@mailinator.com</t>
+  </si>
+  <si>
+    <t>Candidate Password</t>
+  </si>
+  <si>
+    <t>wipro@mailinator.com</t>
+  </si>
+  <si>
+    <t>source1@mailinator.com</t>
+  </si>
+  <si>
+    <t>automate@workstreets.com</t>
+  </si>
+  <si>
+    <t>CorpDashGS</t>
+  </si>
+  <si>
+    <t>CorpDashGO</t>
+  </si>
+  <si>
+    <t>Active JDs - 28; Profiles Received - 92; Expenses - 780000</t>
+  </si>
+  <si>
+    <t>Offered - 10; Onboarded - 10; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>152</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>182</t>
-  </si>
-  <si>
-    <t>192</t>
-  </si>
-  <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>206</t>
-  </si>
-  <si>
-    <t>209</t>
-  </si>
-  <si>
-    <t>211</t>
-  </si>
-  <si>
-    <t>212</t>
-  </si>
-  <si>
-    <t>246</t>
-  </si>
-  <si>
-    <t>366</t>
+    <t>216</t>
+  </si>
+  <si>
+    <t>Active JDs - 29; Profiles Received - 93; Expenses - 790000</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t>223</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>Active JDs - 30; Profiles Received - 94; Expenses - 800000</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>229</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>232</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
+    <t>Active JDs - 31; Profiles Received - 95; Expenses - 810000</t>
+  </si>
+  <si>
+    <t>Offered - 11; Onboarded - 11; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>235</t>
+  </si>
+  <si>
+    <t>Active JDs - 32; Profiles Received - 96; Expenses - 820000</t>
+  </si>
+  <si>
+    <t>Offered - 12; Onboarded - 12; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>Active JDs - 33; Profiles Received - 109; Expenses - 840000</t>
+  </si>
+  <si>
+    <t>Offered - 14; Onboarded - 14; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>Active JDs - 33; Profiles Received - 110; Expenses - 870000</t>
+  </si>
+  <si>
+    <t>Active JDs - 34; Profiles Received - 121; Expenses - 880000</t>
+  </si>
+  <si>
+    <t>Offered - 15; Onboarded - 15; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>Active JDs - 35; Profiles Received - 144; Expenses - 907500</t>
+  </si>
+  <si>
+    <t>Active JDs - 36; Profiles Received - 182; Expenses - 935000</t>
+  </si>
+  <si>
+    <t>350</t>
+  </si>
+  <si>
+    <t>354</t>
+  </si>
+  <si>
+    <t>Active JDs - 37; Profiles Received - 183; Expenses - 945000</t>
+  </si>
+  <si>
+    <t>Offered - 16; Onboarded - 16; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>355</t>
+  </si>
+  <si>
+    <t>356</t>
+  </si>
+  <si>
+    <t>Active JDs - 38; Profiles Received - 184; Expenses - 955000</t>
+  </si>
+  <si>
+    <t>357</t>
+  </si>
+  <si>
+    <t>358</t>
+  </si>
+  <si>
+    <t>Active JDs - 39; Profiles Received - 185; Expenses - 965000</t>
+  </si>
+  <si>
+    <t>Offered - 17; Onboarded - 17; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>359</t>
+  </si>
+  <si>
+    <t>360</t>
+  </si>
+  <si>
+    <t>Active JDs - 40; Profiles Received - 189; Expenses - 975000</t>
+  </si>
+  <si>
+    <t>Offered - 18; Onboarded - 18; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>361</t>
+  </si>
+  <si>
+    <t>362</t>
+  </si>
+  <si>
+    <t>Active JDs - 41; Profiles Received - 190; Expenses - 985000</t>
+  </si>
+  <si>
+    <t>363</t>
+  </si>
+  <si>
+    <t>365</t>
+  </si>
+  <si>
+    <t>368</t>
+  </si>
+  <si>
+    <t>372</t>
+  </si>
+  <si>
+    <t>390</t>
+  </si>
+  <si>
+    <t>393</t>
+  </si>
+  <si>
+    <t>Active JDs - 42; Profiles Received - 190; Expenses - 1012500</t>
+  </si>
+  <si>
+    <t>426</t>
+  </si>
+  <si>
+    <t>427</t>
+  </si>
+  <si>
+    <t>428</t>
+  </si>
+  <si>
+    <t>429</t>
+  </si>
+  <si>
+    <t>Active JDs - 43; Profiles Received - 191; Expenses - 1022500</t>
+  </si>
+  <si>
+    <t>430</t>
+  </si>
+  <si>
+    <t>431</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t>433</t>
+  </si>
+  <si>
+    <t>Active JDs - 44; Profiles Received - 192; Expenses - 1032500</t>
+  </si>
+  <si>
+    <t>Offered - 21; Onboarded - 21; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>434</t>
+  </si>
+  <si>
+    <t>435</t>
+  </si>
+  <si>
+    <t>Active JDs - 45; Profiles Received - 193; Expenses - 1042500</t>
+  </si>
+  <si>
+    <t>Offered - 22; Onboarded - 22; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>443</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>451</t>
+  </si>
+  <si>
+    <t>457</t>
+  </si>
+  <si>
+    <t>458</t>
+  </si>
+  <si>
+    <t>Active JDs - 46; Profiles Received - 195; Expenses - 1062500</t>
+  </si>
+  <si>
+    <t>470</t>
+  </si>
+  <si>
+    <t>471</t>
+  </si>
+  <si>
+    <t>472</t>
+  </si>
+  <si>
+    <t>473</t>
   </si>
 </sst>
 </file>
@@ -646,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +909,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,15 +922,15 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>0</v>
@@ -710,17 +938,33 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="7" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>0</v>
       </c>
     </row>
@@ -730,10 +974,12 @@
     <hyperlink r:id="rId2" ref="B2"/>
     <hyperlink r:id="rId3" ref="B4"/>
     <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
+    <hyperlink r:id="rId5" ref="B7"/>
+    <hyperlink r:id="rId6" ref="B8"/>
+    <hyperlink r:id="rId7" ref="B9"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -775,7 +1021,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1039,9 +1285,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1072,10 +1318,26 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified for the current changes 06Feb19
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="2" windowHeight="3540" windowWidth="12000" xWindow="0" yWindow="2445"/>
+    <workbookView windowHeight="6915" windowWidth="14940" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" r:id="rId1" sheetId="1"/>
@@ -14,7 +14,7 @@
     <sheet name="Write data" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K16"/>
+  <oleSize ref="A1:J21"/>
 </workbook>
 </file>
 
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
   <si>
     <t>admin@123</t>
   </si>
@@ -238,250 +238,52 @@
     <t>CorpDashGO</t>
   </si>
   <si>
-    <t>Active JDs - 28; Profiles Received - 92; Expenses - 780000</t>
-  </si>
-  <si>
-    <t>Offered - 10; Onboarded - 10; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>152</t>
+    <t>Active JDs - 55; Profiles Received - 217; Expenses - 1236250</t>
+  </si>
+  <si>
+    <t>Offered - 24; Onboarded - 23; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>552</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>216</t>
-  </si>
-  <si>
-    <t>Active JDs - 29; Profiles Received - 93; Expenses - 790000</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>221</t>
-  </si>
-  <si>
-    <t>223</t>
-  </si>
-  <si>
-    <t>224</t>
-  </si>
-  <si>
-    <t>226</t>
-  </si>
-  <si>
-    <t>227</t>
-  </si>
-  <si>
-    <t>Active JDs - 30; Profiles Received - 94; Expenses - 800000</t>
-  </si>
-  <si>
-    <t>228</t>
-  </si>
-  <si>
-    <t>229</t>
-  </si>
-  <si>
-    <t>230</t>
-  </si>
-  <si>
-    <t>231</t>
-  </si>
-  <si>
-    <t>232</t>
-  </si>
-  <si>
-    <t>233</t>
-  </si>
-  <si>
-    <t>Active JDs - 31; Profiles Received - 95; Expenses - 810000</t>
-  </si>
-  <si>
-    <t>Offered - 11; Onboarded - 11; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>234</t>
-  </si>
-  <si>
-    <t>235</t>
-  </si>
-  <si>
-    <t>Active JDs - 32; Profiles Received - 96; Expenses - 820000</t>
-  </si>
-  <si>
-    <t>Offered - 12; Onboarded - 12; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>Active JDs - 33; Profiles Received - 109; Expenses - 840000</t>
-  </si>
-  <si>
-    <t>Offered - 14; Onboarded - 14; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>Active JDs - 33; Profiles Received - 110; Expenses - 870000</t>
-  </si>
-  <si>
-    <t>Active JDs - 34; Profiles Received - 121; Expenses - 880000</t>
-  </si>
-  <si>
-    <t>Offered - 15; Onboarded - 15; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>Active JDs - 35; Profiles Received - 144; Expenses - 907500</t>
-  </si>
-  <si>
-    <t>Active JDs - 36; Profiles Received - 182; Expenses - 935000</t>
-  </si>
-  <si>
-    <t>350</t>
-  </si>
-  <si>
-    <t>354</t>
-  </si>
-  <si>
-    <t>Active JDs - 37; Profiles Received - 183; Expenses - 945000</t>
-  </si>
-  <si>
-    <t>Offered - 16; Onboarded - 16; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>355</t>
-  </si>
-  <si>
-    <t>356</t>
-  </si>
-  <si>
-    <t>Active JDs - 38; Profiles Received - 184; Expenses - 955000</t>
-  </si>
-  <si>
-    <t>357</t>
-  </si>
-  <si>
-    <t>358</t>
-  </si>
-  <si>
-    <t>Active JDs - 39; Profiles Received - 185; Expenses - 965000</t>
-  </si>
-  <si>
-    <t>Offered - 17; Onboarded - 17; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>359</t>
-  </si>
-  <si>
-    <t>360</t>
-  </si>
-  <si>
-    <t>Active JDs - 40; Profiles Received - 189; Expenses - 975000</t>
-  </si>
-  <si>
-    <t>Offered - 18; Onboarded - 18; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>361</t>
-  </si>
-  <si>
-    <t>362</t>
-  </si>
-  <si>
-    <t>Active JDs - 41; Profiles Received - 190; Expenses - 985000</t>
-  </si>
-  <si>
-    <t>363</t>
-  </si>
-  <si>
-    <t>365</t>
-  </si>
-  <si>
-    <t>368</t>
-  </si>
-  <si>
-    <t>372</t>
-  </si>
-  <si>
-    <t>390</t>
-  </si>
-  <si>
-    <t>393</t>
-  </si>
-  <si>
-    <t>Active JDs - 42; Profiles Received - 190; Expenses - 1012500</t>
-  </si>
-  <si>
-    <t>426</t>
-  </si>
-  <si>
-    <t>427</t>
-  </si>
-  <si>
-    <t>428</t>
-  </si>
-  <si>
-    <t>429</t>
-  </si>
-  <si>
-    <t>Active JDs - 43; Profiles Received - 191; Expenses - 1022500</t>
-  </si>
-  <si>
-    <t>430</t>
-  </si>
-  <si>
-    <t>431</t>
-  </si>
-  <si>
-    <t>432</t>
-  </si>
-  <si>
-    <t>433</t>
-  </si>
-  <si>
-    <t>Active JDs - 44; Profiles Received - 192; Expenses - 1032500</t>
-  </si>
-  <si>
-    <t>Offered - 21; Onboarded - 21; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>434</t>
-  </si>
-  <si>
-    <t>435</t>
-  </si>
-  <si>
-    <t>Active JDs - 45; Profiles Received - 193; Expenses - 1042500</t>
-  </si>
-  <si>
-    <t>Offered - 22; Onboarded - 22; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>443</t>
-  </si>
-  <si>
-    <t>444</t>
-  </si>
-  <si>
-    <t>451</t>
-  </si>
-  <si>
-    <t>457</t>
-  </si>
-  <si>
-    <t>458</t>
-  </si>
-  <si>
-    <t>Active JDs - 46; Profiles Received - 195; Expenses - 1062500</t>
-  </si>
-  <si>
-    <t>470</t>
-  </si>
-  <si>
-    <t>471</t>
-  </si>
-  <si>
-    <t>472</t>
-  </si>
-  <si>
-    <t>473</t>
+    <t>Active JDs - 56; Profiles Received - 218; Expenses - 1246250</t>
+  </si>
+  <si>
+    <t>573</t>
+  </si>
+  <si>
+    <t>Active JDs - 58; Profiles Received - 221; Expenses - 1283750</t>
+  </si>
+  <si>
+    <t>Offered - 25; Onboarded - 23; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>580</t>
+  </si>
+  <si>
+    <t>Active JDs - 66; Profiles Received - 238; Expenses - 1323750</t>
+  </si>
+  <si>
+    <t>611</t>
+  </si>
+  <si>
+    <t>614</t>
+  </si>
+  <si>
+    <t>Active JDs - 67; Profiles Received - 240; Expenses - 1333750</t>
+  </si>
+  <si>
+    <t>618</t>
+  </si>
+  <si>
+    <t>617</t>
+  </si>
+  <si>
+    <t>621</t>
   </si>
 </sst>
 </file>
@@ -876,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,7 +1089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1321,7 +1123,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1329,7 +1131,7 @@
         <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1337,7 +1139,7 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 25 Change Correction and Agent Assign Candidates Test cases
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="72">
   <si>
     <t>admin@123</t>
   </si>
@@ -226,79 +226,49 @@
     <t>source1@mailinator.com</t>
   </si>
   <si>
-    <t>automate@workstreets.com</t>
-  </si>
-  <si>
     <t>CorpDashGS</t>
   </si>
   <si>
     <t>CorpDashGO</t>
   </si>
   <si>
-    <t>Active JDs - 67; Profiles Received - 240; Expenses - 1333750</t>
-  </si>
-  <si>
-    <t>Offered - 27; Onboarded - 25; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>623</t>
-  </si>
-  <si>
-    <t>c@nada.email</t>
+    <t>Offered - 4; Onboarded - 4; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>Active JDs - 82; Profiles Received - 84; Expenses - 830000</t>
+  </si>
+  <si>
+    <t>1223</t>
+  </si>
+  <si>
+    <t>wipro@mailinator.com</t>
+  </si>
+  <si>
+    <t>adminsiva@nada.email</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Active JDs - 0; Profiles Received - 0; Expenses - 0</t>
-  </si>
-  <si>
-    <t>Offered - 0; Onboarded - 0; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>640</t>
-  </si>
-  <si>
-    <t>653</t>
-  </si>
-  <si>
-    <t>655</t>
-  </si>
-  <si>
-    <t>666</t>
-  </si>
-  <si>
-    <t>670</t>
-  </si>
-  <si>
-    <t>676</t>
-  </si>
-  <si>
-    <t>678</t>
-  </si>
-  <si>
-    <t>688</t>
-  </si>
-  <si>
-    <t>696</t>
-  </si>
-  <si>
-    <t>710</t>
-  </si>
-  <si>
-    <t>715</t>
-  </si>
-  <si>
-    <t>719</t>
-  </si>
-  <si>
-    <t>722</t>
-  </si>
-  <si>
-    <t>724</t>
-  </si>
-  <si>
-    <t>725</t>
+    <t>Active JDs - 93; Profiles Received - 317; Expenses - 1518750</t>
+  </si>
+  <si>
+    <t>Offered - 28; Onboarded - 26; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t>1228</t>
+  </si>
+  <si>
+    <t>1233</t>
+  </si>
+  <si>
+    <t>1235</t>
+  </si>
+  <si>
+    <t>Active JDs - 94; Profiles Received - 318; Expenses - 1528750</t>
+  </si>
+  <si>
+    <t>1238</t>
   </si>
 </sst>
 </file>
@@ -694,7 +664,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +696,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -742,7 +712,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1138,20 +1108,20 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Corrected for Failed Testcases
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="3220" windowWidth="9960" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9960" windowHeight="3220"/>
   </bookViews>
   <sheets>
-    <sheet name="Login Page" r:id="rId1" sheetId="1"/>
-    <sheet name="Job Summary page" r:id="rId2" sheetId="2"/>
-    <sheet name="Add Skills page" r:id="rId3" sheetId="3"/>
-    <sheet name="Update Before Execution" r:id="rId4" sheetId="4"/>
-    <sheet name="Write data" r:id="rId5" sheetId="5"/>
+    <sheet name="Login Page" sheetId="1" r:id="rId1"/>
+    <sheet name="Job Summary page" sheetId="2" r:id="rId2"/>
+    <sheet name="Add Skills page" sheetId="3" r:id="rId3"/>
+    <sheet name="Update Before Execution" sheetId="4" r:id="rId4"/>
+    <sheet name="Write data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:J21"/>
@@ -24,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>admin@123</t>
   </si>
@@ -232,41 +232,25 @@
     <t>wipro@mailinator.com</t>
   </si>
   <si>
-    <t>adminsiva@nada.email</t>
-  </si>
-  <si>
-    <t>Offered - 29; Onboarded - 27; TotalMoneySaved - 0</t>
-  </si>
-  <si>
     <t>1335</t>
   </si>
   <si>
-    <t>Active JDs - 103; Profiles Received - 352; Expenses - 1906250</t>
-  </si>
-  <si>
     <t>barish@nada.email</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Active JDs - 103; Profiles Received - 352; Expenses - 1916250</t>
-  </si>
-  <si>
-    <t>Active JDs - 103; Profiles Received - 352; Expenses - 1926250</t>
-  </si>
-  <si>
     <t>Active JDs - 103; Profiles Received - 356; Expenses - Coming Soon</t>
   </si>
   <si>
-    <t>Offered - 29; Onboarded - 27; TotalMoneySaved - Coming Soon</t>
+    <t>Offered - 0; Onboarded - 0; TotalMoneySaved - Coming Soon</t>
+  </si>
+  <si>
+    <t>automate@workstreets.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -335,28 +319,28 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -373,10 +357,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -411,7 +395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,7 +430,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -534,7 +518,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -543,13 +527,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -559,7 +543,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -568,7 +552,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -577,7 +561,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -587,12 +571,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -623,7 +607,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -642,7 +626,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -654,18 +638,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.54296875" collapsed="true"/>
-    <col min="3" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -706,7 +690,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -738,7 +722,7 @@
         <v>53</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -751,22 +735,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B3"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B7"/>
-    <hyperlink r:id="rId6" ref="B8"/>
-    <hyperlink r:id="rId7" ref="B9"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId8"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -774,10 +758,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -858,14 +842,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -970,7 +954,7 @@
         <v>37</v>
       </c>
     </row>
-    <row ht="15" r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -978,7 +962,7 @@
         <v>43</v>
       </c>
     </row>
-    <row ht="15" r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -986,7 +970,7 @@
         <v>12</v>
       </c>
     </row>
-    <row ht="15" r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -994,7 +978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row ht="15" r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1002,7 +986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row ht="15" r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1011,13 +995,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
@@ -1025,10 +1009,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.54296875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1058,15 +1042,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1074,10 +1058,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.54296875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1102,7 +1086,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1110,7 +1094,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1118,10 +1102,10 @@
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Smoke Test Failures
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19290" windowHeight="6780" firstSheet="2" activeTab="2"/>
+    <workbookView activeTab="2" firstSheet="2" windowHeight="6780" windowWidth="19290"/>
   </bookViews>
   <sheets>
-    <sheet name="Login Page" sheetId="1" r:id="rId1"/>
-    <sheet name="Job Summary page" sheetId="2" r:id="rId2"/>
-    <sheet name="Add Skills page" sheetId="3" r:id="rId3"/>
-    <sheet name="Update Before Execution" sheetId="4" r:id="rId4"/>
-    <sheet name="Write data" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="Login Page" r:id="rId1" sheetId="1"/>
+    <sheet name="Job Summary page" r:id="rId2" sheetId="2"/>
+    <sheet name="Add Skills page" r:id="rId3" sheetId="3"/>
+    <sheet name="Update Before Execution" r:id="rId4" sheetId="4"/>
+    <sheet name="Write data" r:id="rId5" sheetId="5"/>
+    <sheet name="Sheet1" r:id="rId6" sheetId="6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:J21"/>
@@ -25,7 +25,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment authorId="0" ref="B2">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="3">
   <si>
     <t>Key</t>
   </si>
@@ -520,6 +520,15 @@
   </si>
   <si>
     <t>Offered - 29; Onboarded - 27; TotalMoneySaved - 0</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Active JDs - 103; Profiles Received - 356; Expenses - Coming Soon</t>
+  </si>
+  <si>
+    <t>Offered - 0; Onboarded - 0; TotalMoneySaved - Coming Soon</t>
   </si>
 </sst>
 </file>
@@ -1014,216 +1023,216 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="179">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="178">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="7" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="24" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="23" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="10" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="27" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="19" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="19" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="26" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="33" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="25" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="30" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="29" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="32" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="31" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="28" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="3" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="10" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+  <cellXfs count="9">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="10"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="10"/>
+    <xf applyAlignment="1" applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="10"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
+    <cellStyle builtinId="10" name="Note" xfId="9"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1237,10 +1246,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1398,7 +1407,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1407,13 +1416,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1423,7 +1432,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1432,7 +1441,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1441,7 +1450,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1451,12 +1460,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1487,7 +1496,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1506,7 +1515,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1517,9 +1526,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -1527,9 +1536,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="28.5714285714286" customWidth="1"/>
-    <col min="3" max="5" width="14.1428571428571" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.5714285714286" collapsed="true"/>
+    <col min="3" max="5" customWidth="true" width="14.1428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1615,35 +1624,35 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="admin@123"/>
-    <hyperlink ref="B2" r:id="rId2" display="wipro@mailinator.com"/>
-    <hyperlink ref="B4" r:id="rId3" display="adminsiva@nada.email"/>
-    <hyperlink ref="B5" r:id="rId1" display="admin@123"/>
-    <hyperlink ref="B7" r:id="rId1" display="admin@123"/>
-    <hyperlink ref="B8" r:id="rId4" display="barish@nada.email" tooltip="mailto:barish@nada.email"/>
-    <hyperlink ref="B9" r:id="rId1" display="admin@123"/>
+    <hyperlink display="admin@123" r:id="rId1" ref="B3"/>
+    <hyperlink display="wipro@mailinator.com" r:id="rId2" ref="B2"/>
+    <hyperlink display="adminsiva@nada.email" r:id="rId3" ref="B4"/>
+    <hyperlink display="admin@123" r:id="rId1" ref="B5"/>
+    <hyperlink display="admin@123" r:id="rId1" ref="B7"/>
+    <hyperlink display="barish@nada.email" r:id="rId4" ref="B8" tooltip="mailto:barish@nada.email"/>
+    <hyperlink display="admin@123" r:id="rId1" ref="B9"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="16.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="25.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="17.4285714285714" customWidth="1"/>
-    <col min="4" max="5" width="14.1428571428571" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.5714285714286" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.8571428571429" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.4285714285714" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="14.1428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1724,16 +1733,16 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <headerFooter/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B57"/>
@@ -2277,26 +2286,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="26.2857142857143" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.5714285714286" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="14.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.2857142857143" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.5714285714286" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.5714285714286" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="14.1428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2326,28 +2335,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="register@mailinator.com"/>
+    <hyperlink display="register@mailinator.com" r:id="rId1" ref="B2"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" width="26.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="19.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="25.5714285714286" customWidth="1"/>
-    <col min="4" max="5" width="14.1428571428571" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="26.2857142857143" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.5714285714286" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.5714285714286" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" width="14.1428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2380,7 +2389,7 @@
         <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2388,17 +2397,17 @@
         <v>154</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
   <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -2408,7 +2417,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageMargins bottom="1" footer="0.511805555555556" header="0.511805555555556" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Candidate_TC006, TC013, TC014 ,WSAdmin_TC30
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="3630" windowWidth="10575" xWindow="0" yWindow="2445"/>
+    <workbookView xWindow="0" yWindow="2450" windowWidth="10580" windowHeight="3630"/>
   </bookViews>
   <sheets>
-    <sheet name="Login Page" r:id="rId1" sheetId="1"/>
-    <sheet name="Job Summary page" r:id="rId2" sheetId="2"/>
-    <sheet name="Add Skills page" r:id="rId3" sheetId="3"/>
-    <sheet name="Update Before Execution" r:id="rId4" sheetId="4"/>
-    <sheet name="Write data" r:id="rId5" sheetId="5"/>
+    <sheet name="Login Page" sheetId="1" r:id="rId1"/>
+    <sheet name="Job Summary page" sheetId="2" r:id="rId2"/>
+    <sheet name="Add Skills page" sheetId="3" r:id="rId3"/>
+    <sheet name="Update Before Execution" sheetId="4" r:id="rId4"/>
+    <sheet name="Write data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J21"/>
 </workbook>
 </file>
 
@@ -24,7 +23,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="B2">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
   <si>
     <t>admin@123</t>
   </si>
@@ -217,9 +216,6 @@
     <t>Candidate Email</t>
   </si>
   <si>
-    <t>sathish@mailinator.com</t>
-  </si>
-  <si>
     <t>Candidate Password</t>
   </si>
   <si>
@@ -232,80 +228,37 @@
     <t>CorpDashGO</t>
   </si>
   <si>
-    <t>Offered - 4; Onboarded - 4; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>Active JDs - 82; Profiles Received - 84; Expenses - 830000</t>
-  </si>
-  <si>
-    <t>1223</t>
-  </si>
-  <si>
     <t>wipro@mailinator.com</t>
   </si>
   <si>
     <t>adminsiva@nada.email</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Active JDs - 93; Profiles Received - 317; Expenses - 1518750</t>
-  </si>
-  <si>
-    <t>Offered - 28; Onboarded - 26; TotalMoneySaved - 0</t>
-  </si>
-  <si>
-    <t>1228</t>
-  </si>
-  <si>
-    <t>1233</t>
-  </si>
-  <si>
-    <t>1235</t>
-  </si>
-  <si>
-    <t>Active JDs - 94; Profiles Received - 318; Expenses - 1528750</t>
-  </si>
-  <si>
-    <t>1238</t>
-  </si>
-  <si>
-    <t>1239</t>
-  </si>
-  <si>
-    <t>1244</t>
-  </si>
-  <si>
-    <t>1245</t>
-  </si>
-  <si>
-    <t>1246</t>
-  </si>
-  <si>
-    <t>1254</t>
-  </si>
-  <si>
-    <t>Active JDs - 97; Profiles Received - 321; Expenses - 1558750</t>
-  </si>
-  <si>
     <t>Offered - 29; Onboarded - 27; TotalMoneySaved - 0</t>
   </si>
   <si>
-    <t>1255</t>
-  </si>
-  <si>
     <t>Active JDs - 103; Profiles Received - 345; Expenses - 1618750</t>
   </si>
   <si>
     <t>1335</t>
+  </si>
+  <si>
+    <t>automate@workstreets.com</t>
+  </si>
+  <si>
+    <t>Super Admin Email</t>
+  </si>
+  <si>
+    <t>Super Admin Pwd</t>
+  </si>
+  <si>
+    <t>can06@mailinator.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,31 +327,34 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -409,10 +365,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -447,7 +403,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -482,7 +438,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,7 +526,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -579,13 +535,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -595,7 +551,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -604,7 +560,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -613,7 +569,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -623,12 +579,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -659,7 +615,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -678,7 +634,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -690,21 +646,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="3" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -721,15 +677,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -737,15 +693,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -753,15 +709,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -769,54 +725,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>55</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B3"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B7"/>
-    <hyperlink r:id="rId6" ref="B8"/>
-    <hyperlink r:id="rId7" ref="B9"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId8"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -833,7 +807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -841,7 +815,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -849,7 +823,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -860,7 +834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -871,7 +845,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -882,7 +856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -894,22 +868,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -926,7 +900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -934,7 +908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -942,7 +916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -950,7 +924,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -958,7 +932,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -966,7 +940,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -974,7 +948,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -982,7 +956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -990,7 +964,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -998,7 +972,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1006,7 +980,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1014,7 +988,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1022,7 +996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1030,7 +1004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1038,7 +1012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1047,27 +1021,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1084,7 +1058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1094,29 +1068,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1133,31 +1107,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>57</v>
       </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected for Super Admin
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="3220" windowWidth="9960" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9960" windowHeight="3220"/>
   </bookViews>
   <sheets>
-    <sheet name="Login Page" r:id="rId1" sheetId="1"/>
-    <sheet name="Job Summary page" r:id="rId2" sheetId="2"/>
-    <sheet name="Add Skills page" r:id="rId3" sheetId="3"/>
-    <sheet name="Update Before Execution" r:id="rId4" sheetId="4"/>
-    <sheet name="Write data" r:id="rId5" sheetId="5"/>
+    <sheet name="Login Page" sheetId="1" r:id="rId1"/>
+    <sheet name="Job Summary page" sheetId="2" r:id="rId2"/>
+    <sheet name="Add Skills page" sheetId="3" r:id="rId3"/>
+    <sheet name="Update Before Execution" sheetId="4" r:id="rId4"/>
+    <sheet name="Write data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J21"/>
 </workbook>
 </file>
 
@@ -24,7 +23,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>admin@123</t>
   </si>
@@ -247,14 +246,16 @@
     <t>automate@workstreets.com</t>
   </si>
   <si>
-    <t/>
+    <t>Super Admin Email</t>
+  </si>
+  <si>
+    <t>Super Admin Pwd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -323,28 +324,28 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -361,10 +362,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -399,7 +400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -434,7 +435,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,7 +523,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -531,13 +532,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -547,7 +548,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -556,7 +557,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -565,7 +566,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -575,12 +576,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -611,7 +612,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -630,7 +631,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -642,18 +643,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.54296875" collapsed="true"/>
-    <col min="3" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -737,24 +738,42 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B3"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B7"/>
-    <hyperlink r:id="rId6" ref="B8"/>
-    <hyperlink r:id="rId7" ref="B9"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId8"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -762,10 +781,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -846,14 +865,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -958,7 +977,7 @@
         <v>37</v>
       </c>
     </row>
-    <row ht="15" r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -966,7 +985,7 @@
         <v>43</v>
       </c>
     </row>
-    <row ht="15" r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -974,7 +993,7 @@
         <v>12</v>
       </c>
     </row>
-    <row ht="15" r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -982,7 +1001,7 @@
         <v>14</v>
       </c>
     </row>
-    <row ht="15" r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -990,7 +1009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row ht="15" r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -999,13 +1018,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
@@ -1013,10 +1032,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.54296875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1046,15 +1065,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1062,10 +1081,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.54296875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1110,6 +1129,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CHanged the configuration to Dev environment
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
   <si>
     <t>admin@123</t>
   </si>
@@ -247,7 +247,22 @@
     <t>automate@workstreets.com</t>
   </si>
   <si>
+    <t>corpadmin@nada.email</t>
+  </si>
+  <si>
+    <t>noreply-dev@workstreets.com</t>
+  </si>
+  <si>
+    <t>raagency@nada.email</t>
+  </si>
+  <si>
+    <t>foka@getnada.com</t>
+  </si>
+  <si>
     <t/>
+  </si>
+  <si>
+    <t>Active JDs - 2; Profiles Received - 9; Expenses - Coming Soon</t>
   </si>
 </sst>
 </file>
@@ -645,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,6 +693,9 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -688,12 +706,18 @@
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>63</v>
       </c>
     </row>
@@ -704,12 +728,18 @@
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="C5" s="7" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -720,12 +750,18 @@
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="C7" s="7" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>60</v>
       </c>
     </row>
@@ -734,6 +770,9 @@
         <v>54</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>0</v>
       </c>
     </row>
@@ -746,9 +785,17 @@
     <hyperlink r:id="rId5" ref="B7"/>
     <hyperlink r:id="rId6" ref="B8"/>
     <hyperlink r:id="rId7" ref="B9"/>
+    <hyperlink r:id="rId8" ref="C3"/>
+    <hyperlink r:id="rId9" ref="C2"/>
+    <hyperlink r:id="rId10" ref="C4"/>
+    <hyperlink r:id="rId11" ref="C5"/>
+    <hyperlink r:id="rId12" ref="C7"/>
+    <hyperlink r:id="rId13" ref="C8"/>
+    <hyperlink r:id="rId14" ref="C9"/>
+    <hyperlink r:id="rId15" ref="B6"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId8"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -1098,7 +1145,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fixed Cookies in Develop
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="3220" windowWidth="9960" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9960" windowHeight="3220"/>
   </bookViews>
   <sheets>
-    <sheet name="Login Page" r:id="rId1" sheetId="1"/>
-    <sheet name="Job Summary page" r:id="rId2" sheetId="2"/>
-    <sheet name="Add Skills page" r:id="rId3" sheetId="3"/>
-    <sheet name="Update Before Execution" r:id="rId4" sheetId="4"/>
-    <sheet name="Write data" r:id="rId5" sheetId="5"/>
+    <sheet name="Login Page" sheetId="1" r:id="rId1"/>
+    <sheet name="Job Summary page" sheetId="2" r:id="rId2"/>
+    <sheet name="Add Skills page" sheetId="3" r:id="rId3"/>
+    <sheet name="Update Before Execution" sheetId="4" r:id="rId4"/>
+    <sheet name="Write data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:J21"/>
@@ -24,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>admin@123</t>
   </si>
@@ -238,28 +238,10 @@
     <t>barish@nada.email</t>
   </si>
   <si>
-    <t>Active JDs - 103; Profiles Received - 356; Expenses - Coming Soon</t>
-  </si>
-  <si>
     <t>Offered - 0; Onboarded - 0; TotalMoneySaved - Coming Soon</t>
   </si>
   <si>
     <t>automate@workstreets.com</t>
-  </si>
-  <si>
-    <t>corpadmin@nada.email</t>
-  </si>
-  <si>
-    <t>noreply-dev@workstreets.com</t>
-  </si>
-  <si>
-    <t>raagency@nada.email</t>
-  </si>
-  <si>
-    <t>foka@getnada.com</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Active JDs - 2; Profiles Received - 9; Expenses - Coming Soon</t>
@@ -269,7 +251,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -338,28 +319,28 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -376,10 +357,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -414,7 +395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,7 +430,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -537,7 +518,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -546,13 +527,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -562,7 +543,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -571,7 +552,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -580,7 +561,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -590,12 +571,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -626,7 +607,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -645,7 +626,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -657,18 +638,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.54296875" collapsed="true"/>
-    <col min="3" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -693,11 +674,9 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -706,20 +685,16 @@
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>63</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -728,20 +703,16 @@
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="7" t="s">
         <v>55</v>
       </c>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -750,20 +721,16 @@
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="7" t="s">
         <v>60</v>
       </c>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -772,36 +739,26 @@
       <c r="B9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="C9" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B3"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B7"/>
-    <hyperlink r:id="rId6" ref="B8"/>
-    <hyperlink r:id="rId7" ref="B9"/>
-    <hyperlink r:id="rId8" ref="C3"/>
-    <hyperlink r:id="rId9" ref="C2"/>
-    <hyperlink r:id="rId10" ref="C4"/>
-    <hyperlink r:id="rId11" ref="C5"/>
-    <hyperlink r:id="rId12" ref="C7"/>
-    <hyperlink r:id="rId13" ref="C8"/>
-    <hyperlink r:id="rId14" ref="C9"/>
-    <hyperlink r:id="rId15" ref="B6"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId16"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -809,10 +766,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -893,14 +850,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -1005,7 +962,7 @@
         <v>37</v>
       </c>
     </row>
-    <row ht="15" r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1013,7 +970,7 @@
         <v>43</v>
       </c>
     </row>
-    <row ht="15" r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1021,7 +978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row ht="15" r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1029,7 +986,7 @@
         <v>14</v>
       </c>
     </row>
-    <row ht="15" r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1037,7 +994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row ht="15" r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1046,13 +1003,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
@@ -1060,10 +1017,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.54296875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1093,15 +1050,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1109,10 +1066,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.54296875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1145,7 +1102,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1153,10 +1110,10 @@
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Sprint 30 changes
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView windowHeight="3220" windowWidth="9960" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" windowHeight="3220" windowWidth="9960" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login Page" r:id="rId1" sheetId="1"/>
@@ -14,7 +14,7 @@
     <sheet name="Write data" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J21"/>
+  <oleSize ref="A10:D18"/>
 </workbook>
 </file>
 
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="117">
   <si>
     <t>admin@123</t>
   </si>
@@ -238,22 +238,172 @@
     <t>barish@nada.email</t>
   </si>
   <si>
-    <t>Offered - 0; Onboarded - 0; TotalMoneySaved - Coming Soon</t>
-  </si>
-  <si>
     <t>automate@workstreets.com</t>
   </si>
   <si>
-    <t>Active JDs - 2; Profiles Received - 9; Expenses - Coming Soon</t>
+    <t>Active JDs - 104; Profiles Received - 357; Expenses - Coming Soon</t>
+  </si>
+  <si>
+    <t>Offered - 2; Onboarded - 2; TotalMoneySaved - Coming Soon</t>
+  </si>
+  <si>
+    <t>Super Admin Email</t>
+  </si>
+  <si>
+    <t>Super Admin Pwd</t>
+  </si>
+  <si>
+    <t>skill11</t>
+  </si>
+  <si>
+    <t>skill12</t>
+  </si>
+  <si>
+    <t>skill13</t>
+  </si>
+  <si>
+    <t>skill14</t>
+  </si>
+  <si>
+    <t>skill15</t>
+  </si>
+  <si>
+    <t>skill16</t>
+  </si>
+  <si>
+    <t>skill17</t>
+  </si>
+  <si>
+    <t>skill18</t>
+  </si>
+  <si>
+    <t>skill19</t>
+  </si>
+  <si>
+    <t>skill20</t>
+  </si>
+  <si>
+    <t>skill21</t>
+  </si>
+  <si>
+    <t>skill22</t>
+  </si>
+  <si>
+    <t>skill23</t>
+  </si>
+  <si>
+    <t>skill24</t>
+  </si>
+  <si>
+    <t>skill25</t>
+  </si>
+  <si>
+    <t>skill26</t>
+  </si>
+  <si>
+    <t>skill27</t>
+  </si>
+  <si>
+    <t>skill28</t>
+  </si>
+  <si>
+    <t>skill29</t>
+  </si>
+  <si>
+    <t>skill30</t>
+  </si>
+  <si>
+    <t>skill31</t>
+  </si>
+  <si>
+    <t>skill32</t>
+  </si>
+  <si>
+    <t>skill33</t>
+  </si>
+  <si>
+    <t>skill34</t>
+  </si>
+  <si>
+    <t>skill35</t>
+  </si>
+  <si>
+    <t>skill36</t>
+  </si>
+  <si>
+    <t>skill37</t>
+  </si>
+  <si>
+    <t>skill38</t>
+  </si>
+  <si>
+    <t>skill39</t>
+  </si>
+  <si>
+    <t>skill40</t>
+  </si>
+  <si>
+    <t>skill41</t>
+  </si>
+  <si>
+    <t>skill42</t>
+  </si>
+  <si>
+    <t>skill43</t>
+  </si>
+  <si>
+    <t>skill44</t>
+  </si>
+  <si>
+    <t>skill45</t>
+  </si>
+  <si>
+    <t>skill46</t>
+  </si>
+  <si>
+    <t>skill47</t>
+  </si>
+  <si>
+    <t>skill48</t>
+  </si>
+  <si>
+    <t>skill49</t>
+  </si>
+  <si>
+    <t>skill50</t>
+  </si>
+  <si>
+    <t>skill51</t>
+  </si>
+  <si>
+    <t>skill52</t>
+  </si>
+  <si>
+    <t>skill53</t>
+  </si>
+  <si>
+    <t>skill54</t>
+  </si>
+  <si>
+    <t>skill55</t>
+  </si>
+  <si>
+    <t>skill56</t>
+  </si>
+  <si>
+    <t>skill57</t>
+  </si>
+  <si>
+    <t>skill58</t>
+  </si>
+  <si>
+    <t>skill59</t>
+  </si>
+  <si>
+    <t>skill60</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>Active JDs - 104; Profiles Received - 357; Expenses - Coming Soon</t>
-  </si>
-  <si>
-    <t>Offered - 2; Onboarded - 2; TotalMoneySaved - Coming Soon</t>
   </si>
 </sst>
 </file>
@@ -649,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -702,7 +852,7 @@
         <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="7"/>
     </row>
@@ -750,6 +900,22 @@
         <v>0</v>
       </c>
       <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -760,9 +926,11 @@
     <hyperlink r:id="rId5" ref="B7"/>
     <hyperlink r:id="rId6" ref="B8"/>
     <hyperlink r:id="rId7" ref="B9"/>
+    <hyperlink r:id="rId8" ref="B10"/>
+    <hyperlink r:id="rId9" ref="B11"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId8"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -867,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -964,7 +1132,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -972,43 +1140,443 @@
         <v>37</v>
       </c>
     </row>
-    <row ht="15" r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row customFormat="1" r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row customFormat="1" r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row customFormat="1" r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row customFormat="1" r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row customFormat="1" r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row customFormat="1" r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row customFormat="1" r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row customFormat="1" r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row customFormat="1" r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row customFormat="1" r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row customFormat="1" r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row customFormat="1" r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row customFormat="1" r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row customFormat="1" r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row customFormat="1" r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row customFormat="1" r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row customFormat="1" r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row customFormat="1" r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row customFormat="1" r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row customFormat="1" r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row customFormat="1" r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row customFormat="1" r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row customFormat="1" r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row customFormat="1" r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row customFormat="1" r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row customFormat="1" r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row customFormat="1" r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row customFormat="1" r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row customFormat="1" r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row customFormat="1" r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row customFormat="1" r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row customFormat="1" r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row customFormat="1" r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row customFormat="1" r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row customFormat="1" r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row customFormat="1" r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row customFormat="1" r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row customFormat="1" r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row customFormat="1" r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row customFormat="1" r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row customFormat="1" r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row customFormat="1" r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row customFormat="1" r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row customFormat="1" r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row customFormat="1" r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row customFormat="1" r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row customFormat="1" r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row customFormat="1" r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row customFormat="1" r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row customFormat="1" r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B62" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row ht="15" r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row customFormat="1" r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B63" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row ht="15" r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row customFormat="1" r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B64" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row ht="15" r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row customFormat="1" r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B65" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row ht="15" r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row customFormat="1" r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B66" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1112,7 +1680,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1120,7 +1688,7 @@
         <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WSADM TC023, TC024, TC026
</commit_message>
<xml_diff>
--- a/com.automation.wsp/src/main/resources/TestData.xlsx
+++ b/com.automation.wsp/src/main/resources/TestData.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="3220" windowWidth="9960" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9960" windowHeight="3220"/>
   </bookViews>
   <sheets>
-    <sheet name="Login Page" r:id="rId1" sheetId="1"/>
-    <sheet name="Job Summary page" r:id="rId2" sheetId="2"/>
-    <sheet name="Add Skills page" r:id="rId3" sheetId="3"/>
-    <sheet name="Update Before Execution" r:id="rId4" sheetId="4"/>
-    <sheet name="Write data" r:id="rId5" sheetId="5"/>
+    <sheet name="Login Page" sheetId="1" r:id="rId1"/>
+    <sheet name="Job Summary page" sheetId="2" r:id="rId2"/>
+    <sheet name="Add Skills page" sheetId="3" r:id="rId3"/>
+    <sheet name="Update Before Execution" sheetId="4" r:id="rId4"/>
+    <sheet name="Write data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A10:D18"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -24,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment authorId="0" ref="B2" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="116">
   <si>
     <t>admin@123</t>
   </si>
@@ -401,16 +401,12 @@
   </si>
   <si>
     <t>skill60</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -479,28 +475,28 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -517,10 +513,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -555,7 +551,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -590,7 +586,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -678,7 +674,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -687,13 +683,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -703,7 +699,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -712,7 +708,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -721,7 +717,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -731,12 +727,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -767,7 +763,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -786,7 +782,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -798,18 +794,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.54296875" collapsed="true"/>
-    <col min="3" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -919,24 +915,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B3"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B7"/>
-    <hyperlink r:id="rId6" ref="B8"/>
-    <hyperlink r:id="rId7" ref="B9"/>
-    <hyperlink r:id="rId8" ref="B10"/>
-    <hyperlink r:id="rId9" ref="B11"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="B10" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId10"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -944,10 +940,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1028,17 +1024,17 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1132,7 +1128,7 @@
         <v>36</v>
       </c>
     </row>
-    <row customFormat="1" r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1140,7 +1136,7 @@
         <v>37</v>
       </c>
     </row>
-    <row customFormat="1" r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -1148,7 +1144,7 @@
         <v>66</v>
       </c>
     </row>
-    <row customFormat="1" r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -1156,7 +1152,7 @@
         <v>67</v>
       </c>
     </row>
-    <row customFormat="1" r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -1164,7 +1160,7 @@
         <v>68</v>
       </c>
     </row>
-    <row customFormat="1" r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -1172,7 +1168,7 @@
         <v>69</v>
       </c>
     </row>
-    <row customFormat="1" r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -1180,7 +1176,7 @@
         <v>70</v>
       </c>
     </row>
-    <row customFormat="1" r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -1188,7 +1184,7 @@
         <v>71</v>
       </c>
     </row>
-    <row customFormat="1" r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -1196,7 +1192,7 @@
         <v>72</v>
       </c>
     </row>
-    <row customFormat="1" r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -1204,7 +1200,7 @@
         <v>73</v>
       </c>
     </row>
-    <row customFormat="1" r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -1212,7 +1208,7 @@
         <v>74</v>
       </c>
     </row>
-    <row customFormat="1" r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -1220,7 +1216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row customFormat="1" r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -1228,7 +1224,7 @@
         <v>76</v>
       </c>
     </row>
-    <row customFormat="1" r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1236,7 +1232,7 @@
         <v>77</v>
       </c>
     </row>
-    <row customFormat="1" r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -1244,7 +1240,7 @@
         <v>78</v>
       </c>
     </row>
-    <row customFormat="1" r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -1252,7 +1248,7 @@
         <v>79</v>
       </c>
     </row>
-    <row customFormat="1" r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -1260,7 +1256,7 @@
         <v>80</v>
       </c>
     </row>
-    <row customFormat="1" r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -1268,7 +1264,7 @@
         <v>81</v>
       </c>
     </row>
-    <row customFormat="1" r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -1276,7 +1272,7 @@
         <v>82</v>
       </c>
     </row>
-    <row customFormat="1" r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1284,7 +1280,7 @@
         <v>83</v>
       </c>
     </row>
-    <row customFormat="1" r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -1292,7 +1288,7 @@
         <v>84</v>
       </c>
     </row>
-    <row customFormat="1" r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -1300,7 +1296,7 @@
         <v>85</v>
       </c>
     </row>
-    <row customFormat="1" r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>86</v>
       </c>
@@ -1308,7 +1304,7 @@
         <v>86</v>
       </c>
     </row>
-    <row customFormat="1" r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>87</v>
       </c>
@@ -1316,7 +1312,7 @@
         <v>87</v>
       </c>
     </row>
-    <row customFormat="1" r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -1324,7 +1320,7 @@
         <v>88</v>
       </c>
     </row>
-    <row customFormat="1" r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -1332,7 +1328,7 @@
         <v>89</v>
       </c>
     </row>
-    <row customFormat="1" r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>90</v>
       </c>
@@ -1340,7 +1336,7 @@
         <v>90</v>
       </c>
     </row>
-    <row customFormat="1" r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -1348,7 +1344,7 @@
         <v>91</v>
       </c>
     </row>
-    <row customFormat="1" r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>92</v>
       </c>
@@ -1356,7 +1352,7 @@
         <v>92</v>
       </c>
     </row>
-    <row customFormat="1" r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>93</v>
       </c>
@@ -1364,7 +1360,7 @@
         <v>93</v>
       </c>
     </row>
-    <row customFormat="1" r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -1372,7 +1368,7 @@
         <v>94</v>
       </c>
     </row>
-    <row customFormat="1" r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -1380,7 +1376,7 @@
         <v>95</v>
       </c>
     </row>
-    <row customFormat="1" r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -1388,7 +1384,7 @@
         <v>96</v>
       </c>
     </row>
-    <row customFormat="1" r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>97</v>
       </c>
@@ -1396,7 +1392,7 @@
         <v>97</v>
       </c>
     </row>
-    <row customFormat="1" r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -1404,7 +1400,7 @@
         <v>98</v>
       </c>
     </row>
-    <row customFormat="1" r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>99</v>
       </c>
@@ -1412,7 +1408,7 @@
         <v>99</v>
       </c>
     </row>
-    <row customFormat="1" r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -1420,7 +1416,7 @@
         <v>100</v>
       </c>
     </row>
-    <row customFormat="1" r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -1428,7 +1424,7 @@
         <v>101</v>
       </c>
     </row>
-    <row customFormat="1" r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -1436,7 +1432,7 @@
         <v>102</v>
       </c>
     </row>
-    <row customFormat="1" r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>103</v>
       </c>
@@ -1444,7 +1440,7 @@
         <v>103</v>
       </c>
     </row>
-    <row customFormat="1" r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>104</v>
       </c>
@@ -1452,7 +1448,7 @@
         <v>104</v>
       </c>
     </row>
-    <row customFormat="1" r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -1460,7 +1456,7 @@
         <v>105</v>
       </c>
     </row>
-    <row customFormat="1" r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>106</v>
       </c>
@@ -1468,7 +1464,7 @@
         <v>106</v>
       </c>
     </row>
-    <row customFormat="1" r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -1476,7 +1472,7 @@
         <v>107</v>
       </c>
     </row>
-    <row customFormat="1" r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>108</v>
       </c>
@@ -1484,7 +1480,7 @@
         <v>108</v>
       </c>
     </row>
-    <row customFormat="1" r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -1492,7 +1488,7 @@
         <v>109</v>
       </c>
     </row>
-    <row customFormat="1" r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -1500,7 +1496,7 @@
         <v>110</v>
       </c>
     </row>
-    <row customFormat="1" r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>111</v>
       </c>
@@ -1508,7 +1504,7 @@
         <v>111</v>
       </c>
     </row>
-    <row customFormat="1" r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -1516,7 +1512,7 @@
         <v>112</v>
       </c>
     </row>
-    <row customFormat="1" r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>113</v>
       </c>
@@ -1524,7 +1520,7 @@
         <v>113</v>
       </c>
     </row>
-    <row customFormat="1" r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>114</v>
       </c>
@@ -1532,7 +1528,7 @@
         <v>114</v>
       </c>
     </row>
-    <row customFormat="1" r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>115</v>
       </c>
@@ -1540,7 +1536,7 @@
         <v>115</v>
       </c>
     </row>
-    <row customFormat="1" r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>38</v>
       </c>
@@ -1548,7 +1544,7 @@
         <v>43</v>
       </c>
     </row>
-    <row customFormat="1" r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>39</v>
       </c>
@@ -1556,7 +1552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row customFormat="1" r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>40</v>
       </c>
@@ -1564,7 +1560,7 @@
         <v>14</v>
       </c>
     </row>
-    <row customFormat="1" r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>41</v>
       </c>
@@ -1572,7 +1568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row customFormat="1" r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -1581,13 +1577,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
@@ -1595,10 +1591,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.54296875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1628,15 +1624,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -1644,10 +1640,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.54296875" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
+    <col min="1" max="1" width="26.26953125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1692,6 +1688,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>